<commit_message>
Fixes in serialing and qty 0 when box breaking fix has been done
</commit_message>
<xml_diff>
--- a/wwwroot/27/ExtrasCalculation.xlsx
+++ b/wwwroot/27/ExtrasCalculation.xlsx
@@ -59,7 +59,7 @@
     <t>10195</t>
   </si>
   <si>
-    <t>04-10-2024</t>
+    <t>10-04-2024</t>
   </si>
   <si>
     <t>07:00 AM to 10:00 AM</t>
@@ -77,13 +77,13 @@
     <t>10196</t>
   </si>
   <si>
-    <t>04-12-2024</t>
+    <t>12-04-2024</t>
   </si>
   <si>
     <t>10204</t>
   </si>
   <si>
-    <t>04-09-2024</t>
+    <t>09-04-2024</t>
   </si>
   <si>
     <t>11:00 AM to 02:00 PM</t>
@@ -158,7 +158,7 @@
     <t>11003</t>
   </si>
   <si>
-    <t>04-08-2024</t>
+    <t>08-04-2024</t>
   </si>
   <si>
     <t>11004</t>

</xml_diff>